<commit_message>
se eliminan imgs sobrantes, se testea nueva seccion en index quote y lista
</commit_message>
<xml_diff>
--- a/assets/txts/gant_proyecto_portafolio.xlsx
+++ b/assets/txts/gant_proyecto_portafolio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rodrigoquiroz/Desktop/portafolio/assets/txts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BD5E6F-A5E1-DA44-AEC2-304E3850B971}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A36CB1A7-C9E9-A041-9777-88F0F5E1B32B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7240" yWindow="1080" windowWidth="31100" windowHeight="22320" xr2:uid="{60A37438-1DA6-3149-A875-4B26474D580D}"/>
+    <workbookView xWindow="27920" yWindow="1560" windowWidth="23280" windowHeight="24480" xr2:uid="{60A37438-1DA6-3149-A875-4B26474D580D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
   <si>
     <t xml:space="preserve">estado </t>
   </si>
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t xml:space="preserve">Forkeos a dos repos </t>
-  </si>
-  <si>
-    <t>commit</t>
   </si>
   <si>
     <t>Check de reuqrimientos examen</t>
@@ -131,6 +128,27 @@
   </si>
   <si>
     <t>Edición de imágenes e incorporación al sitio</t>
+  </si>
+  <si>
+    <t>forkeo repo en user de github (seccion repositorios)</t>
+  </si>
+  <si>
+    <t>abro carpeta de proyecto en visual studio code</t>
+  </si>
+  <si>
+    <t>en terminal de carpeta padre escribo git clone + enlace ssh que obtengo del repo forkeado</t>
+  </si>
+  <si>
+    <t>en terminal  cd a carpeta del proyecto ya clonado</t>
+  </si>
+  <si>
+    <t>abro el archivo a modificar (html / css / img) hago cambios en index o css</t>
+  </si>
+  <si>
+    <t>git add . &gt; git commit -m "" &gt; git log &gt; git push origin master / main (según lo que indique la consola)</t>
+  </si>
+  <si>
+    <t>chekeo en repo forkeado</t>
   </si>
 </sst>
 </file>
@@ -198,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -210,11 +228,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -231,10 +252,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -534,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D92F35B5-581B-2747-BFA2-64700B268A4D}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -550,11 +567,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -606,8 +623,8 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="26" x14ac:dyDescent="0.35">
-      <c r="A5" s="8" t="s">
-        <v>28</v>
+      <c r="A5" s="7" t="s">
+        <v>27</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
@@ -616,13 +633,15 @@
         <v>7</v>
       </c>
       <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="E5" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" ht="26" x14ac:dyDescent="0.35">
-      <c r="A6" s="8"/>
+      <c r="A6" s="7"/>
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
@@ -630,13 +649,15 @@
         <v>7</v>
       </c>
       <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="E6" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" ht="26" x14ac:dyDescent="0.35">
-      <c r="A7" s="8"/>
+      <c r="A7" s="7"/>
       <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
@@ -644,13 +665,15 @@
         <v>7</v>
       </c>
       <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="E7" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="26" x14ac:dyDescent="0.35">
-      <c r="A8" s="8"/>
+      <c r="A8" s="7"/>
       <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
@@ -658,169 +681,214 @@
         <v>7</v>
       </c>
       <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="E8" s="4"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" ht="26" x14ac:dyDescent="0.35">
-      <c r="A9" s="8"/>
+      <c r="A9" s="7"/>
       <c r="B9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="E9" s="4"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" ht="26" x14ac:dyDescent="0.35">
-      <c r="A10" s="8"/>
+      <c r="A10" s="7"/>
       <c r="B10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="E10" s="4"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" ht="47" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="6" t="s">
-        <v>16</v>
+      <c r="A11" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" ht="26" x14ac:dyDescent="0.35">
-      <c r="A12" s="6"/>
+      <c r="A12" s="8"/>
       <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>17</v>
-      </c>
+      <c r="C12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="4"/>
     </row>
     <row r="13" spans="1:8" ht="26" x14ac:dyDescent="0.35">
-      <c r="A13" s="6"/>
+      <c r="A13" s="8"/>
       <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="26" x14ac:dyDescent="0.35">
-      <c r="A14" s="6"/>
+      <c r="C13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="54" x14ac:dyDescent="0.35">
+      <c r="A14" s="8"/>
       <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="26" x14ac:dyDescent="0.35">
+      <c r="C14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="E15" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="26" x14ac:dyDescent="0.35">
+      <c r="A16" s="6"/>
+      <c r="B16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="E16" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="37" x14ac:dyDescent="0.35">
+      <c r="A17" s="6"/>
+      <c r="B17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" ht="37" x14ac:dyDescent="0.35">
+      <c r="A18" s="6"/>
+      <c r="B18" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" ht="37" x14ac:dyDescent="0.35">
+      <c r="A19" s="6"/>
+      <c r="B19" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" ht="26" x14ac:dyDescent="0.35">
+      <c r="B20" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="1:4" ht="37" x14ac:dyDescent="0.35">
+      <c r="A21" s="1"/>
+      <c r="B21" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="1:4" ht="37" x14ac:dyDescent="0.35">
+      <c r="A22" s="1"/>
+      <c r="B22" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:4" ht="26" x14ac:dyDescent="0.35">
+      <c r="A23" s="1"/>
+      <c r="B23" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="1:4" ht="37" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" spans="1:4" ht="26" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="26" x14ac:dyDescent="0.35">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="37" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="26" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="1:4" ht="26" x14ac:dyDescent="0.35">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="1:4" ht="26" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="26" x14ac:dyDescent="0.35">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="1:4" ht="26" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="1:4" ht="26" x14ac:dyDescent="0.35">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="4"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
+      <c r="C27" s="1"/>
+      <c r="D27" s="4"/>
+    </row>
+    <row r="28" spans="1:4" ht="26" x14ac:dyDescent="0.35">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
cambia navbar, se corrigen links y se arregla menu hamburguesa
</commit_message>
<xml_diff>
--- a/assets/txts/gant_proyecto_portafolio.xlsx
+++ b/assets/txts/gant_proyecto_portafolio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rodrigoquiroz/Desktop/portafolio/assets/txts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A36CB1A7-C9E9-A041-9777-88F0F5E1B32B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{491584B4-491E-4E47-B1FD-DEC9EBD96A1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27920" yWindow="1560" windowWidth="23280" windowHeight="24480" xr2:uid="{60A37438-1DA6-3149-A875-4B26474D580D}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="26960" xr2:uid="{60A37438-1DA6-3149-A875-4B26474D580D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="41">
   <si>
     <t xml:space="preserve">estado </t>
   </si>
@@ -67,15 +67,6 @@
   </si>
   <si>
     <t>Desafio Surfon_Cupon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forkeos a dos repos </t>
-  </si>
-  <si>
-    <t>Check de reuqrimientos examen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">detalle </t>
   </si>
   <si>
     <t>direccionamiento links nav bar / cómo se hace anchor a partes del portafolio, sapear trabajo de roberto de guiro</t>
@@ -121,12 +112,6 @@
     <t>Bonus track El Fuego</t>
   </si>
   <si>
-    <t>ideas sitio enchuado</t>
-  </si>
-  <si>
-    <t>frase &gt; skills &gt; link a inkdin</t>
-  </si>
-  <si>
     <t>Edición de imágenes e incorporación al sitio</t>
   </si>
   <si>
@@ -149,6 +134,39 @@
   </si>
   <si>
     <t>chekeo en repo forkeado</t>
+  </si>
+  <si>
+    <t>ojo con archivo readme de home</t>
+  </si>
+  <si>
+    <t xml:space="preserve">debe contener descripción de proyecto y direcciones de los repos forkeados </t>
+  </si>
+  <si>
+    <t>Fork a repo 1</t>
+  </si>
+  <si>
+    <t>Fork a repo 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Detalles diseño y pg </t>
+  </si>
+  <si>
+    <t>cambio de color y color bg secciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">incorporación de sección quote al home con su respectivo estilo </t>
+  </si>
+  <si>
+    <t>incorporación de info conocimientos y sofwares a sección sobre mi</t>
+  </si>
+  <si>
+    <t>Check de requerimientos examen</t>
+  </si>
+  <si>
+    <t>git a todo</t>
+  </si>
+  <si>
+    <t>check menu hamburguesa / cuando collapsa no muestra links</t>
   </si>
 </sst>
 </file>
@@ -184,7 +202,7 @@
       <name val="Futura Medium"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -203,6 +221,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -216,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -224,6 +248,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -237,6 +264,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -551,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D92F35B5-581B-2747-BFA2-64700B268A4D}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24:C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -567,11 +595,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -623,8 +651,8 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="26" x14ac:dyDescent="0.35">
-      <c r="A5" s="7" t="s">
-        <v>27</v>
+      <c r="A5" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
@@ -634,14 +662,14 @@
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" ht="26" x14ac:dyDescent="0.35">
-      <c r="A6" s="7"/>
+      <c r="A6" s="8"/>
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
@@ -650,14 +678,14 @@
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" ht="26" x14ac:dyDescent="0.35">
-      <c r="A7" s="7"/>
+      <c r="A7" s="8"/>
       <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
@@ -666,14 +694,14 @@
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="26" x14ac:dyDescent="0.35">
-      <c r="A8" s="7"/>
+      <c r="A8" s="8"/>
       <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
@@ -687,9 +715,9 @@
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" ht="26" x14ac:dyDescent="0.35">
-      <c r="A9" s="7"/>
+      <c r="A9" s="8"/>
       <c r="B9" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>7</v>
@@ -701,9 +729,9 @@
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" ht="26" x14ac:dyDescent="0.35">
-      <c r="A10" s="7"/>
+      <c r="A10" s="8"/>
       <c r="B10" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>7</v>
@@ -715,8 +743,8 @@
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" ht="47" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="8" t="s">
-        <v>15</v>
+      <c r="A11" s="9" t="s">
+        <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>6</v>
@@ -731,7 +759,7 @@
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" ht="26" x14ac:dyDescent="0.35">
-      <c r="A12" s="8"/>
+      <c r="A12" s="9"/>
       <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
@@ -741,7 +769,7 @@
       <c r="E12" s="4"/>
     </row>
     <row r="13" spans="1:8" ht="26" x14ac:dyDescent="0.35">
-      <c r="A13" s="8"/>
+      <c r="A13" s="9"/>
       <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
@@ -749,11 +777,11 @@
         <v>7</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="54" x14ac:dyDescent="0.35">
-      <c r="A14" s="8"/>
+      <c r="A14" s="9"/>
       <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
@@ -761,134 +789,299 @@
         <v>7</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="E15" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="26" x14ac:dyDescent="0.35">
       <c r="A16" s="6"/>
       <c r="B16" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="3"/>
+        <v>24</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="E16" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="37" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="37" x14ac:dyDescent="0.35">
       <c r="A17" s="6"/>
       <c r="B17" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="3"/>
-    </row>
-    <row r="18" spans="1:4" ht="37" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="37" x14ac:dyDescent="0.35">
       <c r="A18" s="6"/>
       <c r="B18" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="3"/>
-    </row>
-    <row r="19" spans="1:4" ht="37" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="37" x14ac:dyDescent="0.35">
       <c r="A19" s="6"/>
       <c r="B19" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="3"/>
-    </row>
-    <row r="20" spans="1:4" ht="26" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="26" x14ac:dyDescent="0.35">
       <c r="B20" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="1:4" ht="37" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="37" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="1"/>
-    </row>
-    <row r="22" spans="1:4" ht="37" x14ac:dyDescent="0.35">
+        <v>27</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="37" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="1"/>
-    </row>
-    <row r="23" spans="1:4" ht="26" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="26" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="26" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="3"/>
+    </row>
+    <row r="25" spans="1:3" ht="26" x14ac:dyDescent="0.35">
+      <c r="A25" s="7"/>
+      <c r="B25" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="3"/>
+    </row>
+    <row r="26" spans="1:3" ht="37" x14ac:dyDescent="0.35">
+      <c r="A26" s="7"/>
+      <c r="B26" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="3"/>
+    </row>
+    <row r="27" spans="1:3" ht="37" x14ac:dyDescent="0.35">
+      <c r="A27" s="7"/>
+      <c r="B27" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="3"/>
+    </row>
+    <row r="28" spans="1:3" ht="37" x14ac:dyDescent="0.35">
+      <c r="A28" s="7"/>
+      <c r="B28" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="3"/>
+    </row>
+    <row r="29" spans="1:3" ht="26" x14ac:dyDescent="0.35">
+      <c r="B29" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="3"/>
+    </row>
+    <row r="30" spans="1:3" ht="37" x14ac:dyDescent="0.35">
+      <c r="A30" s="1"/>
+      <c r="B30" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" s="3"/>
+    </row>
+    <row r="31" spans="1:3" ht="37" x14ac:dyDescent="0.35">
+      <c r="A31" s="1"/>
+      <c r="B31" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="3"/>
+    </row>
+    <row r="32" spans="1:3" ht="26" x14ac:dyDescent="0.35">
+      <c r="A32" s="1"/>
+      <c r="B32" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" s="3"/>
+    </row>
+    <row r="33" spans="1:4" ht="26" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="1"/>
-    </row>
-    <row r="24" spans="1:4" ht="37" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-    </row>
-    <row r="25" spans="1:4" ht="26" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-    </row>
-    <row r="26" spans="1:4" ht="26" x14ac:dyDescent="0.35">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="4"/>
-    </row>
-    <row r="27" spans="1:4" ht="26" x14ac:dyDescent="0.35">
-      <c r="A27" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="4"/>
-    </row>
-    <row r="28" spans="1:4" ht="26" x14ac:dyDescent="0.35">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="4"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
+      <c r="B33" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="37" x14ac:dyDescent="0.35">
+      <c r="A34" s="1"/>
+      <c r="B34" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="37" x14ac:dyDescent="0.35">
+      <c r="A35" s="1"/>
+      <c r="B35" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="37" x14ac:dyDescent="0.35">
+      <c r="A36" s="1"/>
+      <c r="B36" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="37" x14ac:dyDescent="0.35">
+      <c r="A37" s="1"/>
+      <c r="B37" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37" s="11"/>
+    </row>
+    <row r="38" spans="1:4" ht="26" x14ac:dyDescent="0.35">
+      <c r="A38" s="1"/>
+      <c r="B38" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38" s="1"/>
+    </row>
+    <row r="39" spans="1:4" ht="26" x14ac:dyDescent="0.35">
+      <c r="A39" s="1"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="1"/>
+    </row>
+    <row r="40" spans="1:4" ht="26" x14ac:dyDescent="0.35">
+      <c r="A40" s="1"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="1"/>
+    </row>
+    <row r="41" spans="1:4" ht="26" x14ac:dyDescent="0.35">
+      <c r="A41" s="1"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="1"/>
+    </row>
+    <row r="42" spans="1:4" ht="26" x14ac:dyDescent="0.35">
+      <c r="A42" s="1"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="1"/>
+    </row>
+    <row r="43" spans="1:4" ht="26" x14ac:dyDescent="0.35">
+      <c r="A43" s="1"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="1"/>
+    </row>
+    <row r="44" spans="1:4" ht="26" x14ac:dyDescent="0.35">
+      <c r="A44" s="1"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="1"/>
+    </row>
+    <row r="45" spans="1:4" ht="26" x14ac:dyDescent="0.35">
+      <c r="A45" s="1"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="1"/>
+    </row>
+    <row r="46" spans="1:4" ht="37" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+    </row>
+    <row r="47" spans="1:4" ht="26" x14ac:dyDescent="0.35">
+      <c r="A47" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+    </row>
+    <row r="48" spans="1:4" ht="26" x14ac:dyDescent="0.35">
+      <c r="A48" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C48" s="1"/>
+      <c r="D48" s="4"/>
+    </row>
+    <row r="49" spans="1:4" ht="26" x14ac:dyDescent="0.35">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="4"/>
+    </row>
+    <row r="50" spans="1:4" ht="26" x14ac:dyDescent="0.35">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="4"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="4"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
se actualiza README con repos forkeados y gantt de proyecto
</commit_message>
<xml_diff>
--- a/assets/txts/gant_proyecto_portafolio.xlsx
+++ b/assets/txts/gant_proyecto_portafolio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rodrigoquiroz/Desktop/portafolio/assets/txts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{491584B4-491E-4E47-B1FD-DEC9EBD96A1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26943EE6-5C47-F440-A611-517BFB89CA93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="26960" xr2:uid="{60A37438-1DA6-3149-A875-4B26474D580D}"/>
+    <workbookView xWindow="28220" yWindow="1620" windowWidth="21040" windowHeight="21700" xr2:uid="{60A37438-1DA6-3149-A875-4B26474D580D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="47">
   <si>
     <t xml:space="preserve">estado </t>
   </si>
@@ -167,6 +167,24 @@
   </si>
   <si>
     <t>check menu hamburguesa / cuando collapsa no muestra links</t>
+  </si>
+  <si>
+    <t>ok / me ayudó el profe</t>
+  </si>
+  <si>
+    <t>https://github.com/RodDev88/desafio1_jbenvenu</t>
+  </si>
+  <si>
+    <t>https://github.com/RodDev88/Desafio1_lau</t>
+  </si>
+  <si>
+    <t>subirlo a github con todo el proceso git</t>
+  </si>
+  <si>
+    <t>url a compartir en examen</t>
+  </si>
+  <si>
+    <t>https://roddev88.github.io/</t>
   </si>
 </sst>
 </file>
@@ -579,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D92F35B5-581B-2747-BFA2-64700B268A4D}">
-  <dimension ref="A1:H53"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24:C32"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -881,75 +899,91 @@
       </c>
     </row>
     <row r="24" spans="1:3" ht="26" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="11" t="s">
         <v>33</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="3"/>
+      <c r="C24" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="25" spans="1:3" ht="26" x14ac:dyDescent="0.35">
       <c r="A25" s="7"/>
       <c r="B25" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="3"/>
+      <c r="C25" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="26" spans="1:3" ht="37" x14ac:dyDescent="0.35">
       <c r="A26" s="7"/>
       <c r="B26" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="3"/>
-    </row>
-    <row r="27" spans="1:3" ht="37" x14ac:dyDescent="0.35">
-      <c r="A27" s="7"/>
+      <c r="C26" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="26" x14ac:dyDescent="0.35">
       <c r="B27" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C27" s="3"/>
+        <v>26</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="28" spans="1:3" ht="37" x14ac:dyDescent="0.35">
-      <c r="A28" s="7"/>
+      <c r="A28" s="1"/>
       <c r="B28" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C28" s="3"/>
-    </row>
-    <row r="29" spans="1:3" ht="26" x14ac:dyDescent="0.35">
+        <v>27</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="37" x14ac:dyDescent="0.35">
+      <c r="A29" s="1"/>
       <c r="B29" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C29" s="3"/>
-    </row>
-    <row r="30" spans="1:3" ht="37" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="26" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
       <c r="B30" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C30" s="3"/>
     </row>
-    <row r="31" spans="1:3" ht="37" x14ac:dyDescent="0.35">
-      <c r="A31" s="1"/>
+    <row r="31" spans="1:3" ht="26" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="B31" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C31" s="3"/>
-    </row>
-    <row r="32" spans="1:3" ht="26" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="37" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
       <c r="B32" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C32" s="3"/>
-    </row>
-    <row r="33" spans="1:4" ht="26" x14ac:dyDescent="0.35">
-      <c r="A33" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="37" x14ac:dyDescent="0.35">
+      <c r="A33" s="1"/>
       <c r="B33" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>7</v>
@@ -958,7 +992,7 @@
     <row r="34" spans="1:4" ht="37" x14ac:dyDescent="0.35">
       <c r="A34" s="1"/>
       <c r="B34" s="5" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>7</v>
@@ -967,121 +1001,83 @@
     <row r="35" spans="1:4" ht="37" x14ac:dyDescent="0.35">
       <c r="A35" s="1"/>
       <c r="B35" s="5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="37" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="26" x14ac:dyDescent="0.35">
       <c r="A36" s="1"/>
       <c r="B36" s="5" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="37" x14ac:dyDescent="0.35">
-      <c r="A37" s="1"/>
-      <c r="B37" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C37" s="11"/>
-    </row>
-    <row r="38" spans="1:4" ht="26" x14ac:dyDescent="0.35">
-      <c r="A38" s="1"/>
+    <row r="37" spans="1:4" ht="26" x14ac:dyDescent="0.35">
+      <c r="A37" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" s="1"/>
+      <c r="C37" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="37" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="B38" s="5" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C38" s="1"/>
+      <c r="D38" s="4"/>
     </row>
     <row r="39" spans="1:4" ht="26" x14ac:dyDescent="0.35">
       <c r="A39" s="1"/>
-      <c r="B39" s="5"/>
+      <c r="B39" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="C39" s="1"/>
+      <c r="D39" s="4"/>
     </row>
     <row r="40" spans="1:4" ht="26" x14ac:dyDescent="0.35">
       <c r="A40" s="1"/>
-      <c r="B40" s="5"/>
+      <c r="B40" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="C40" s="1"/>
-    </row>
-    <row r="41" spans="1:4" ht="26" x14ac:dyDescent="0.35">
-      <c r="A41" s="1"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="1"/>
-    </row>
-    <row r="42" spans="1:4" ht="26" x14ac:dyDescent="0.35">
-      <c r="A42" s="1"/>
-      <c r="B42" s="5"/>
-      <c r="C42" s="1"/>
-    </row>
-    <row r="43" spans="1:4" ht="26" x14ac:dyDescent="0.35">
-      <c r="A43" s="1"/>
-      <c r="B43" s="5"/>
-      <c r="C43" s="1"/>
-    </row>
-    <row r="44" spans="1:4" ht="26" x14ac:dyDescent="0.35">
-      <c r="A44" s="1"/>
-      <c r="B44" s="5"/>
-      <c r="C44" s="1"/>
-    </row>
-    <row r="45" spans="1:4" ht="26" x14ac:dyDescent="0.35">
-      <c r="A45" s="1"/>
-      <c r="B45" s="5"/>
-      <c r="C45" s="1"/>
-    </row>
-    <row r="46" spans="1:4" ht="37" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-    </row>
-    <row r="47" spans="1:4" ht="26" x14ac:dyDescent="0.35">
-      <c r="A47" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-    </row>
-    <row r="48" spans="1:4" ht="26" x14ac:dyDescent="0.35">
-      <c r="A48" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C48" s="1"/>
-      <c r="D48" s="4"/>
-    </row>
-    <row r="49" spans="1:4" ht="26" x14ac:dyDescent="0.35">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="4"/>
-    </row>
-    <row r="50" spans="1:4" ht="26" x14ac:dyDescent="0.35">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="4"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="4"/>
-      <c r="B51" s="4"/>
-      <c r="C51" s="4"/>
-      <c r="D51" s="4"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="4"/>
-      <c r="B52" s="4"/>
-      <c r="C52" s="4"/>
-      <c r="D52" s="4"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="4"/>
-      <c r="B53" s="4"/>
-      <c r="C53" s="4"/>
-      <c r="D53" s="4"/>
+      <c r="D40" s="4"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44" t="s">
+        <v>46</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>